<commit_message>
planilha de teste atualizada
</commit_message>
<xml_diff>
--- a/Unidade 4/Guia de testes.xlsx
+++ b/Unidade 4/Guia de testes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spies\Documents\DispositivosMoveis\DPM_2020-1_Equipe_01\Unidade 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73B84D19-224E-4F59-875D-F140FEC9CCA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9610786C-715C-43BA-90B4-B652E194AE98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DB0C1833-B727-4E3B-9C0F-6FC44AE5F3E5}"/>
+    <workbookView xWindow="-19320" yWindow="-60" windowWidth="19440" windowHeight="15000" xr2:uid="{DB0C1833-B727-4E3B-9C0F-6FC44AE5F3E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Ação</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>Mais de um usuário em um mesmo depósito</t>
+  </si>
+  <si>
+    <t>Não atendido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Por termos uma liguagem hibrida tinhamos o interesse de fazer os testes nas duas plataformas. Com o tempo de teste curto, o tempo para a criação de ambiente em um emulador de IOS e a adaptação do códova nesse ambiente nos custaria um tempo de dedicação maior, optamos por deixar o sistema somente em android, visto que ali a aplicação estava estavel. </t>
   </si>
 </sst>
 </file>
@@ -298,22 +304,40 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -334,16 +358,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -355,10 +369,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -661,125 +671,127 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="40.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.453125" customWidth="1"/>
-    <col min="3" max="3" width="18.36328125" customWidth="1"/>
+    <col min="3" max="3" width="64.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4"/>
+      <c r="B2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="6"/>
+      <c r="B3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="6"/>
+      <c r="B4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="11"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="6"/>
+      <c r="B5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="11"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="6"/>
+      <c r="B6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="11"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="6"/>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="11"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="6"/>
+      <c r="B8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="11"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="6"/>
+      <c r="B9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="11"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="6"/>
+      <c r="B10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="11"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="7" t="s">
+      <c r="B11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="11"/>
+    </row>
+    <row r="12" spans="1:3" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="9"/>
+      <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B12">

</xml_diff>